<commit_message>
update import pembayaran manual
</commit_message>
<xml_diff>
--- a/uploads/finance/Template_import_pembayaran_manual.xlsx
+++ b/uploads/finance/Template_import_pembayaran_manual.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NIM</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>NAMA</t>
+  </si>
+  <si>
+    <t>Invoice</t>
   </si>
 </sst>
 </file>
@@ -64,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -87,13 +90,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -376,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -394,6 +411,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>